<commit_message>
working on the selenium
</commit_message>
<xml_diff>
--- a/Data Analytics Bootcamp/Bootcamp syllabus.xlsx
+++ b/Data Analytics Bootcamp/Bootcamp syllabus.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="87" documentId="8_{AA4D1368-67E0-4DCF-803D-4094AD3B16A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFF0BC51-62D0-44C1-9982-2BED5B4ECFD4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A29991F7-3938-4AA6-AD37-AE8F8930D842}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21570" windowHeight="11220" xr2:uid="{A29991F7-3938-4AA6-AD37-AE8F8930D842}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Analytics Bootcamp" sheetId="1" r:id="rId1"/>
@@ -757,23 +757,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -782,9 +779,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1103,8 +1103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4357D5CC-8A1C-4AB4-9245-DC3F4E7EA6CC}">
   <dimension ref="B3:I107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1122,1078 +1122,1091 @@
   <sheetData>
     <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="7" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G5" s="6"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="7" t="s">
+      <c r="H5" s="10"/>
+      <c r="I5" s="3" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="7" t="s">
+      <c r="C6" s="10"/>
+      <c r="D6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="6"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="7" t="s">
+      <c r="H6" s="10"/>
+      <c r="I6" s="3" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="7" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G7" s="6"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="7" t="s">
+      <c r="H7" s="10"/>
+      <c r="I7" s="3" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="7" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G8" s="6"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="7" t="s">
+      <c r="H8" s="10"/>
+      <c r="I8" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="7" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G9" s="6"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="7" t="s">
+      <c r="H9" s="10"/>
+      <c r="I9" s="3" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="7" t="s">
+      <c r="C10" s="10"/>
+      <c r="D10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G10" s="6"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="7" t="s">
+      <c r="H10" s="10"/>
+      <c r="I10" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="7" t="s">
+      <c r="C11" s="10"/>
+      <c r="D11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G11" s="6"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="7" t="s">
+      <c r="H11" s="10"/>
+      <c r="I11" s="3" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G12" s="6"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="7" t="s">
+      <c r="H12" s="10"/>
+      <c r="I12" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="7" t="s">
+      <c r="C13" s="10"/>
+      <c r="D13" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G13" s="6"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="7" t="s">
+      <c r="H13" s="10"/>
+      <c r="I13" s="3" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="7" t="s">
+      <c r="C14" s="10"/>
+      <c r="D14" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="6"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="7" t="s">
+      <c r="H14" s="10"/>
+      <c r="I14" s="3" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="7" t="s">
+      <c r="C15" s="10"/>
+      <c r="D15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G15" s="6"/>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="I15" s="3" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="7" t="s">
+      <c r="C16" s="10"/>
+      <c r="D16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G16" s="6"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="7" t="s">
+      <c r="H16" s="10"/>
+      <c r="I16" s="3" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="7" t="s">
+      <c r="C17" s="10"/>
+      <c r="D17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G17" s="6"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="7" t="s">
+      <c r="H17" s="10"/>
+      <c r="I17" s="3" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="7" t="s">
+      <c r="C18" s="10"/>
+      <c r="D18" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G18" s="6"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="7" t="s">
+      <c r="H18" s="10"/>
+      <c r="I18" s="3" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="7" t="s">
+      <c r="C19" s="10"/>
+      <c r="D19" s="3" t="s">
         <v>18</v>
       </c>
       <c r="G19" s="6"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="7" t="s">
+      <c r="H19" s="10"/>
+      <c r="I19" s="3" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="7" t="s">
+      <c r="C20" s="10"/>
+      <c r="D20" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G20" s="6"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="7" t="s">
+      <c r="H20" s="10"/>
+      <c r="I20" s="3" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="7" t="s">
+      <c r="C21" s="10"/>
+      <c r="D21" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G21" s="6"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="7" t="s">
+      <c r="H21" s="10"/>
+      <c r="I21" s="3" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G22" s="6"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="7" t="s">
+      <c r="H22" s="10"/>
+      <c r="I22" s="3" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="7" t="s">
+      <c r="C23" s="10"/>
+      <c r="D23" s="3" t="s">
         <v>23</v>
       </c>
       <c r="G23" s="6"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="7" t="s">
+      <c r="H23" s="10"/>
+      <c r="I23" s="3" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="7" t="s">
+      <c r="C24" s="10"/>
+      <c r="D24" s="3" t="s">
         <v>24</v>
       </c>
       <c r="G24" s="6"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="7" t="s">
+      <c r="H24" s="10"/>
+      <c r="I24" s="3" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="6"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="7" t="s">
+      <c r="C25" s="10"/>
+      <c r="D25" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G25" s="6"/>
-      <c r="H25" s="2" t="s">
+      <c r="H25" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="I25" s="7" t="s">
+      <c r="I25" s="3" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="6"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="7" t="s">
+      <c r="C26" s="10"/>
+      <c r="D26" s="3" t="s">
         <v>26</v>
       </c>
       <c r="G26" s="6"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="7" t="s">
+      <c r="H26" s="10"/>
+      <c r="I26" s="3" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="6"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="7" t="s">
+      <c r="C27" s="10"/>
+      <c r="D27" s="3" t="s">
         <v>27</v>
       </c>
       <c r="G27" s="6"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="7" t="s">
+      <c r="H27" s="10"/>
+      <c r="I27" s="3" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="6"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="7" t="s">
+      <c r="C28" s="10"/>
+      <c r="D28" s="3" t="s">
         <v>28</v>
       </c>
       <c r="G28" s="6"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="7" t="s">
+      <c r="H28" s="10"/>
+      <c r="I28" s="3" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="6"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="7" t="s">
+      <c r="C29" s="10"/>
+      <c r="D29" s="3" t="s">
         <v>29</v>
       </c>
       <c r="G29" s="6"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="7" t="s">
+      <c r="H29" s="10"/>
+      <c r="I29" s="3" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="6"/>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G30" s="6"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="7" t="s">
+      <c r="H30" s="10"/>
+      <c r="I30" s="3" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="6"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="7" t="s">
+      <c r="C31" s="10"/>
+      <c r="D31" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G31" s="6"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="7" t="s">
+      <c r="H31" s="10"/>
+      <c r="I31" s="3" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="7" t="s">
+      <c r="C32" s="10"/>
+      <c r="D32" s="3" t="s">
         <v>33</v>
       </c>
       <c r="G32" s="6"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="7" t="s">
+      <c r="H32" s="10"/>
+      <c r="I32" s="3" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="6"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="7" t="s">
+      <c r="C33" s="10"/>
+      <c r="D33" s="3" t="s">
         <v>34</v>
       </c>
       <c r="G33" s="6"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="7" t="s">
+      <c r="H33" s="10"/>
+      <c r="I33" s="3" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="6"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="7" t="s">
+      <c r="C34" s="10"/>
+      <c r="D34" s="3" t="s">
         <v>35</v>
       </c>
       <c r="G34" s="6"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="7" t="s">
+      <c r="H34" s="10"/>
+      <c r="I34" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="6"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="7" t="s">
+      <c r="C35" s="10"/>
+      <c r="D35" s="3" t="s">
         <v>36</v>
       </c>
       <c r="G35" s="6"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="7" t="s">
+      <c r="H35" s="10"/>
+      <c r="I35" s="3" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="3" t="s">
         <v>37</v>
       </c>
       <c r="G36" s="6"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="7" t="s">
+      <c r="H36" s="10"/>
+      <c r="I36" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="6"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="7" t="s">
+      <c r="C37" s="10"/>
+      <c r="D37" s="3" t="s">
         <v>38</v>
       </c>
       <c r="G37" s="6"/>
-      <c r="H37" s="2" t="s">
+      <c r="H37" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I37" s="7" t="s">
+      <c r="I37" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="7" t="s">
+      <c r="C38" s="10"/>
+      <c r="D38" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G38" s="6"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="7" t="s">
+      <c r="H38" s="10"/>
+      <c r="I38" s="3" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="6"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="7" t="s">
+      <c r="C39" s="10"/>
+      <c r="D39" s="3" t="s">
         <v>40</v>
       </c>
       <c r="G39" s="6"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="7" t="s">
+      <c r="H39" s="10"/>
+      <c r="I39" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="6"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="7" t="s">
+      <c r="C40" s="10"/>
+      <c r="D40" s="3" t="s">
         <v>41</v>
       </c>
       <c r="G40" s="6"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="7" t="s">
+      <c r="H40" s="10"/>
+      <c r="I40" s="3" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="6"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="7" t="s">
+      <c r="C41" s="10"/>
+      <c r="D41" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G41" s="6"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="7" t="s">
+      <c r="H41" s="10"/>
+      <c r="I41" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="6"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="7" t="s">
+      <c r="C42" s="10"/>
+      <c r="D42" s="3" t="s">
         <v>43</v>
       </c>
       <c r="G42" s="6"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="7" t="s">
+      <c r="H42" s="10"/>
+      <c r="I42" s="3" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="3" t="s">
         <v>45</v>
       </c>
       <c r="G43" s="6"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="7" t="s">
+      <c r="H43" s="10"/>
+      <c r="I43" s="3" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="6"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="7" t="s">
+      <c r="C44" s="10"/>
+      <c r="D44" s="3" t="s">
         <v>46</v>
       </c>
       <c r="G44" s="6"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="7" t="s">
+      <c r="H44" s="10"/>
+      <c r="I44" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="6"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="7" t="s">
+      <c r="C45" s="10"/>
+      <c r="D45" s="3" t="s">
         <v>47</v>
       </c>
       <c r="G45" s="6"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="7" t="s">
+      <c r="H45" s="10"/>
+      <c r="I45" s="3" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="6"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="7" t="s">
+      <c r="C46" s="10"/>
+      <c r="D46" s="3" t="s">
         <v>48</v>
       </c>
       <c r="G46" s="6"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="7" t="s">
+      <c r="H46" s="10"/>
+      <c r="I46" s="3" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="6"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="7" t="s">
+      <c r="C47" s="10"/>
+      <c r="D47" s="3" t="s">
         <v>49</v>
       </c>
       <c r="G47" s="6"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="7" t="s">
+      <c r="H47" s="10"/>
+      <c r="I47" s="3" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="6"/>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="3" t="s">
         <v>52</v>
       </c>
       <c r="G48" s="6"/>
-      <c r="H48" s="2" t="s">
+      <c r="H48" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="I48" s="7" t="s">
+      <c r="I48" s="3" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="6"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="7" t="s">
+      <c r="C49" s="10"/>
+      <c r="D49" s="3" t="s">
         <v>53</v>
       </c>
       <c r="G49" s="6"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="7" t="s">
+      <c r="H49" s="10"/>
+      <c r="I49" s="3" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="6"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="7" t="s">
+      <c r="C50" s="10"/>
+      <c r="D50" s="3" t="s">
         <v>54</v>
       </c>
       <c r="G50" s="6"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="7" t="s">
+      <c r="H50" s="10"/>
+      <c r="I50" s="3" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="6"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="7" t="s">
+      <c r="C51" s="10"/>
+      <c r="D51" s="3" t="s">
         <v>55</v>
       </c>
       <c r="G51" s="6"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="7" t="s">
+      <c r="H51" s="10"/>
+      <c r="I51" s="3" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="6"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="7" t="s">
+      <c r="C52" s="10"/>
+      <c r="D52" s="3" t="s">
         <v>56</v>
       </c>
       <c r="G52" s="6"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="7" t="s">
+      <c r="H52" s="10"/>
+      <c r="I52" s="3" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="6"/>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="3" t="s">
         <v>57</v>
       </c>
       <c r="G53" s="6"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="7" t="s">
+      <c r="H53" s="10"/>
+      <c r="I53" s="3" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="6"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="7" t="s">
+      <c r="C54" s="10"/>
+      <c r="D54" s="3" t="s">
         <v>58</v>
       </c>
       <c r="G54" s="6"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="7" t="s">
+      <c r="H54" s="10"/>
+      <c r="I54" s="3" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="6"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="7" t="s">
+      <c r="C55" s="10"/>
+      <c r="D55" s="3" t="s">
         <v>59</v>
       </c>
       <c r="G55" s="6"/>
-      <c r="H55" s="2" t="s">
+      <c r="H55" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="I55" s="7" t="s">
+      <c r="I55" s="3" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="6"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="7" t="s">
+      <c r="C56" s="10"/>
+      <c r="D56" s="3" t="s">
         <v>60</v>
       </c>
       <c r="G56" s="6"/>
-      <c r="H56" s="2"/>
-      <c r="I56" s="7" t="s">
+      <c r="H56" s="10"/>
+      <c r="I56" s="3" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="6"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="7" t="s">
+      <c r="C57" s="10"/>
+      <c r="D57" s="3" t="s">
         <v>61</v>
       </c>
       <c r="G57" s="6"/>
-      <c r="H57" s="2"/>
-      <c r="I57" s="7" t="s">
+      <c r="H57" s="10"/>
+      <c r="I57" s="3" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="6"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="7" t="s">
+      <c r="C58" s="10"/>
+      <c r="D58" s="3" t="s">
         <v>62</v>
       </c>
       <c r="G58" s="6"/>
-      <c r="H58" s="2"/>
-      <c r="I58" s="7" t="s">
+      <c r="H58" s="10"/>
+      <c r="I58" s="3" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="6"/>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D59" s="7" t="s">
+      <c r="D59" s="3" t="s">
         <v>65</v>
       </c>
       <c r="G59" s="6"/>
-      <c r="H59" s="2"/>
-      <c r="I59" s="7" t="s">
+      <c r="H59" s="10"/>
+      <c r="I59" s="3" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="6"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="7" t="s">
+      <c r="C60" s="10"/>
+      <c r="D60" s="3" t="s">
         <v>66</v>
       </c>
       <c r="G60" s="6"/>
-      <c r="H60" s="2"/>
-      <c r="I60" s="7" t="s">
+      <c r="H60" s="10"/>
+      <c r="I60" s="3" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="6"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="7" t="s">
+      <c r="C61" s="10"/>
+      <c r="D61" s="3" t="s">
         <v>67</v>
       </c>
       <c r="G61" s="6"/>
-      <c r="H61" s="2" t="s">
+      <c r="H61" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="I61" s="7" t="s">
+      <c r="I61" s="3" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="62" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="6"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="7" t="s">
+      <c r="C62" s="10"/>
+      <c r="D62" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G62" s="8"/>
-      <c r="H62" s="9"/>
-      <c r="I62" s="10" t="s">
+      <c r="G62" s="7"/>
+      <c r="H62" s="8"/>
+      <c r="I62" s="4" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="6"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="7" t="s">
+      <c r="C63" s="10"/>
+      <c r="D63" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="6"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="7" t="s">
+      <c r="C64" s="10"/>
+      <c r="D64" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" s="6"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="7" t="s">
+      <c r="C65" s="10"/>
+      <c r="D65" s="3" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="6"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="7" t="s">
+      <c r="C66" s="10"/>
+      <c r="D66" s="3" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="6"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="7" t="s">
+      <c r="C67" s="10"/>
+      <c r="D67" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" s="6"/>
-      <c r="C68" s="2" t="s">
+      <c r="C68" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="D68" s="7" t="s">
+      <c r="D68" s="3" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" s="6"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="7" t="s">
+      <c r="C69" s="10"/>
+      <c r="D69" s="3" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" s="6"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="7" t="s">
+      <c r="C70" s="10"/>
+      <c r="D70" s="3" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="6"/>
-      <c r="C71" s="2"/>
-      <c r="D71" s="7" t="s">
+      <c r="C71" s="10"/>
+      <c r="D71" s="3" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" s="6"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="7" t="s">
+      <c r="C72" s="10"/>
+      <c r="D72" s="3" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" s="6"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="7" t="s">
+      <c r="C73" s="10"/>
+      <c r="D73" s="3" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" s="6"/>
-      <c r="C74" s="2"/>
-      <c r="D74" s="7" t="s">
+      <c r="C74" s="10"/>
+      <c r="D74" s="3" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" s="6"/>
-      <c r="C75" s="2" t="s">
+      <c r="C75" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="D75" s="7" t="s">
+      <c r="D75" s="3" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" s="6"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="7" t="s">
+      <c r="C76" s="10"/>
+      <c r="D76" s="3" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" s="6"/>
-      <c r="C77" s="2"/>
-      <c r="D77" s="7" t="s">
+      <c r="C77" s="10"/>
+      <c r="D77" s="3" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" s="6"/>
-      <c r="C78" s="2"/>
-      <c r="D78" s="7" t="s">
+      <c r="C78" s="10"/>
+      <c r="D78" s="3" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" s="6"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="7" t="s">
+      <c r="C79" s="10"/>
+      <c r="D79" s="3" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" s="6"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="7" t="s">
+      <c r="C80" s="10"/>
+      <c r="D80" s="3" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B81" s="6"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="7" t="s">
+      <c r="C81" s="10"/>
+      <c r="D81" s="3" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B82" s="6"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="7" t="s">
+      <c r="C82" s="10"/>
+      <c r="D82" s="3" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B83" s="6"/>
-      <c r="C83" s="2"/>
-      <c r="D83" s="7" t="s">
+      <c r="C83" s="10"/>
+      <c r="D83" s="3" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B84" s="6"/>
-      <c r="C84" s="2" t="s">
+      <c r="C84" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="D84" s="7" t="s">
+      <c r="D84" s="3" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B85" s="6"/>
-      <c r="C85" s="2"/>
-      <c r="D85" s="7" t="s">
+      <c r="C85" s="10"/>
+      <c r="D85" s="3" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B86" s="6"/>
-      <c r="C86" s="2"/>
-      <c r="D86" s="7" t="s">
+      <c r="C86" s="10"/>
+      <c r="D86" s="3" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B87" s="6"/>
-      <c r="C87" s="2"/>
-      <c r="D87" s="7" t="s">
+      <c r="C87" s="10"/>
+      <c r="D87" s="3" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B88" s="6"/>
-      <c r="C88" s="2"/>
-      <c r="D88" s="7" t="s">
+      <c r="C88" s="10"/>
+      <c r="D88" s="3" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B89" s="6"/>
-      <c r="C89" s="2"/>
-      <c r="D89" s="7" t="s">
+      <c r="C89" s="10"/>
+      <c r="D89" s="3" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B90" s="6"/>
-      <c r="C90" s="2" t="s">
+      <c r="C90" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="D90" s="7" t="s">
+      <c r="D90" s="3" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B91" s="6"/>
-      <c r="C91" s="2"/>
-      <c r="D91" s="7" t="s">
+      <c r="C91" s="10"/>
+      <c r="D91" s="3" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B92" s="6"/>
-      <c r="C92" s="2"/>
-      <c r="D92" s="7" t="s">
+      <c r="C92" s="10"/>
+      <c r="D92" s="3" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" s="6"/>
-      <c r="C93" s="2"/>
-      <c r="D93" s="7" t="s">
+      <c r="C93" s="10"/>
+      <c r="D93" s="3" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B94" s="6"/>
-      <c r="C94" s="2"/>
-      <c r="D94" s="7" t="s">
+      <c r="C94" s="10"/>
+      <c r="D94" s="3" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B95" s="6"/>
-      <c r="C95" s="2"/>
-      <c r="D95" s="7" t="s">
+      <c r="C95" s="10"/>
+      <c r="D95" s="3" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B96" s="6"/>
-      <c r="C96" s="2"/>
-      <c r="D96" s="7" t="s">
+      <c r="C96" s="10"/>
+      <c r="D96" s="3" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" s="6"/>
-      <c r="C97" s="2" t="s">
+      <c r="C97" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="D97" s="7" t="s">
+      <c r="D97" s="3" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B98" s="6"/>
-      <c r="C98" s="2"/>
-      <c r="D98" s="7" t="s">
+      <c r="C98" s="10"/>
+      <c r="D98" s="3" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B99" s="6"/>
-      <c r="C99" s="2"/>
-      <c r="D99" s="7" t="s">
+      <c r="C99" s="10"/>
+      <c r="D99" s="3" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B100" s="6"/>
-      <c r="C100" s="2"/>
-      <c r="D100" s="7" t="s">
+      <c r="C100" s="10"/>
+      <c r="D100" s="3" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B101" s="6"/>
-      <c r="C101" s="2"/>
-      <c r="D101" s="7" t="s">
+      <c r="C101" s="10"/>
+      <c r="D101" s="3" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B102" s="6"/>
-      <c r="C102" s="2"/>
-      <c r="D102" s="7" t="s">
+      <c r="C102" s="10"/>
+      <c r="D102" s="3" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B103" s="6"/>
-      <c r="C103" s="2" t="s">
+      <c r="C103" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="D103" s="7" t="s">
+      <c r="D103" s="3" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B104" s="6"/>
-      <c r="C104" s="2"/>
-      <c r="D104" s="7" t="s">
+      <c r="C104" s="10"/>
+      <c r="D104" s="3" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B105" s="6"/>
-      <c r="C105" s="2"/>
-      <c r="D105" s="7" t="s">
+      <c r="C105" s="10"/>
+      <c r="D105" s="3" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B106" s="6"/>
-      <c r="C106" s="2"/>
-      <c r="D106" s="7" t="s">
+      <c r="C106" s="10"/>
+      <c r="D106" s="3" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="107" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B107" s="8"/>
-      <c r="C107" s="9" t="s">
+      <c r="B107" s="7"/>
+      <c r="C107" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="D107" s="11"/>
+      <c r="D107" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="H55:H60"/>
+    <mergeCell ref="H61:H62"/>
+    <mergeCell ref="C4:C11"/>
+    <mergeCell ref="C12:C21"/>
+    <mergeCell ref="C22:C29"/>
+    <mergeCell ref="C30:C35"/>
+    <mergeCell ref="C36:C42"/>
+    <mergeCell ref="C43:C47"/>
+    <mergeCell ref="H4:H14"/>
+    <mergeCell ref="H15:H24"/>
+    <mergeCell ref="H25:H36"/>
+    <mergeCell ref="H37:H47"/>
+    <mergeCell ref="H48:H54"/>
     <mergeCell ref="B4:B107"/>
     <mergeCell ref="G4:G62"/>
     <mergeCell ref="C107:D107"/>
@@ -2206,19 +2219,6 @@
     <mergeCell ref="C48:C52"/>
     <mergeCell ref="C53:C58"/>
     <mergeCell ref="C59:C67"/>
-    <mergeCell ref="H4:H14"/>
-    <mergeCell ref="H15:H24"/>
-    <mergeCell ref="H25:H36"/>
-    <mergeCell ref="H37:H47"/>
-    <mergeCell ref="H48:H54"/>
-    <mergeCell ref="H55:H60"/>
-    <mergeCell ref="H61:H62"/>
-    <mergeCell ref="C4:C11"/>
-    <mergeCell ref="C12:C21"/>
-    <mergeCell ref="C22:C29"/>
-    <mergeCell ref="C30:C35"/>
-    <mergeCell ref="C36:C42"/>
-    <mergeCell ref="C43:C47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>